<commit_message>
Added 4 new cases
</commit_message>
<xml_diff>
--- a/tools/ExporterSheet.xlsx
+++ b/tools/ExporterSheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6632" uniqueCount="1777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6652" uniqueCount="1783">
   <si>
     <t>NOUMBER</t>
   </si>
@@ -58,13 +58,13 @@
     <t>Automated Messaging Campaigns</t>
   </si>
   <si>
-    <t>NSFW Discord Server Invite</t>
-  </si>
-  <si>
-    <t>Malicious discord server</t>
-  </si>
-  <si>
-    <t>Discord accounts</t>
+    <t>NSFW Discord Invite</t>
+  </si>
+  <si>
+    <t>Discord Servers</t>
+  </si>
+  <si>
+    <t>Discord Accounts</t>
   </si>
   <si>
     <t>Discord</t>
@@ -91,7 +91,7 @@
     <t>Phishing site</t>
   </si>
   <si>
-    <t>Cloned Steam login page</t>
+    <t>Cloned Steam Pages</t>
   </si>
   <si>
     <t>Steam accounts</t>
@@ -127,10 +127,10 @@
     <t>Potential Source of Message</t>
   </si>
   <si>
-    <t>Funpay scam</t>
-  </si>
-  <si>
-    <t>Funpay offer</t>
+    <t>Funpay Fraud</t>
+  </si>
+  <si>
+    <t>Funpay Offers</t>
   </si>
   <si>
     <t>Money</t>
@@ -430,10 +430,10 @@
     <t>тайно дернул</t>
   </si>
   <si>
-    <t>Fake Discord Nitro gift</t>
-  </si>
-  <si>
-    <t>Browser Session Hijacking</t>
+    <t>Fake Nitro Gift</t>
+  </si>
+  <si>
+    <t>Session Hijacking</t>
   </si>
   <si>
     <t>https://shorter.me/discord-nitro</t>
@@ -5342,6 +5342,24 @@
   </si>
   <si>
     <t>https://tinyurl.com/yc7ee3ze</t>
+  </si>
+  <si>
+    <t>1138023535651074070</t>
+  </si>
+  <si>
+    <t>e50ausf.m</t>
+  </si>
+  <si>
+    <t>https://steanmnscommunity.com/105381409</t>
+  </si>
+  <si>
+    <t>691835106565947473</t>
+  </si>
+  <si>
+    <t>blizarice_</t>
+  </si>
+  <si>
+    <t>https://u.to/h-UkIg</t>
   </si>
 </sst>
 </file>
@@ -30822,13 +30840,77 @@
       <c r="A664" s="1">
         <v>663.0</v>
       </c>
-      <c r="C664" s="6"/>
+      <c r="B664" s="2">
+        <v>45728.0</v>
+      </c>
+      <c r="C664" s="3" t="s">
+        <v>1777</v>
+      </c>
+      <c r="D664" s="1" t="s">
+        <v>1778</v>
+      </c>
+      <c r="E664" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F664" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G664" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H664" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I664" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J664" s="4" t="s">
+        <v>1779</v>
+      </c>
+      <c r="K664" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L664" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="665">
       <c r="A665" s="1">
         <v>664.0</v>
       </c>
-      <c r="C665" s="6"/>
+      <c r="B665" s="2">
+        <v>45728.0</v>
+      </c>
+      <c r="C665" s="3" t="s">
+        <v>1780</v>
+      </c>
+      <c r="D665" s="1" t="s">
+        <v>1781</v>
+      </c>
+      <c r="E665" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F665" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G665" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H665" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I665" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J665" s="4" t="s">
+        <v>1782</v>
+      </c>
+      <c r="K665" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L665" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="666">
       <c r="A666" s="1">
@@ -31919,7 +32001,9 @@
     <hyperlink r:id="rId659" ref="J661"/>
     <hyperlink r:id="rId660" ref="J662"/>
     <hyperlink r:id="rId661" ref="J663"/>
+    <hyperlink r:id="rId662" ref="J664"/>
+    <hyperlink r:id="rId663" ref="J665"/>
   </hyperlinks>
-  <drawing r:id="rId662"/>
+  <drawing r:id="rId664"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reverted changes of filepaths in modules
</commit_message>
<xml_diff>
--- a/tools/ExporterSheet.xlsx
+++ b/tools/ExporterSheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6652" uniqueCount="1783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7082" uniqueCount="1852">
   <si>
     <t>NOUMBER</t>
   </si>
@@ -5360,6 +5360,213 @@
   </si>
   <si>
     <t>https://u.to/h-UkIg</t>
+  </si>
+  <si>
+    <t>422088091625586689</t>
+  </si>
+  <si>
+    <t>endershot_1</t>
+  </si>
+  <si>
+    <t>https://in.mt/dVM</t>
+  </si>
+  <si>
+    <t>1038480388110176257</t>
+  </si>
+  <si>
+    <t>migu3lill0rd</t>
+  </si>
+  <si>
+    <t>https://steanmucommunity.com/105952092</t>
+  </si>
+  <si>
+    <t>608571881552871444</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>https://discorb.co/nitro</t>
+  </si>
+  <si>
+    <t>755496074684399718</t>
+  </si>
+  <si>
+    <t>https://discorcl.click/nltro/?=steam</t>
+  </si>
+  <si>
+    <t>675409753500811264</t>
+  </si>
+  <si>
+    <t>https://discordg.link/gift/nitro</t>
+  </si>
+  <si>
+    <t>872619165922512926</t>
+  </si>
+  <si>
+    <t>https://discord.gg/HSZUH6Db3</t>
+  </si>
+  <si>
+    <t>https://discrod-gifts.com/nitro</t>
+  </si>
+  <si>
+    <t>817505845235286066</t>
+  </si>
+  <si>
+    <t>https://discord.gg/pornhub</t>
+  </si>
+  <si>
+    <t>512201835117936650</t>
+  </si>
+  <si>
+    <t>https://discqrde.com/UFDeEmMeCVocD</t>
+  </si>
+  <si>
+    <t>852990385763385374</t>
+  </si>
+  <si>
+    <t>https://discrods.gift/VEBvBmFbECvcW</t>
+  </si>
+  <si>
+    <t>https://discord.gg/myFb9tQ9hW</t>
+  </si>
+  <si>
+    <t>422652692029243392</t>
+  </si>
+  <si>
+    <t>https://rb.gy/7eofb</t>
+  </si>
+  <si>
+    <t>780374628819664916</t>
+  </si>
+  <si>
+    <t>https://discord.gg/sexnudes</t>
+  </si>
+  <si>
+    <t>1068911114622079006</t>
+  </si>
+  <si>
+    <t>https://discord.gg/sexxx</t>
+  </si>
+  <si>
+    <t>568022898447745066</t>
+  </si>
+  <si>
+    <t>https://transfer.sh/get/HfAsYO8EEI/Setup.exe</t>
+  </si>
+  <si>
+    <t>558919553153892353</t>
+  </si>
+  <si>
+    <t>https://discord.gg/ZCnststv6r</t>
+  </si>
+  <si>
+    <t>787946081426079764</t>
+  </si>
+  <si>
+    <t>https://discord.gg/housenudes</t>
+  </si>
+  <si>
+    <t>1116323490736373821</t>
+  </si>
+  <si>
+    <t>842749423805399040</t>
+  </si>
+  <si>
+    <t>https://discord.gg/teennudes</t>
+  </si>
+  <si>
+    <t>921518355540754452</t>
+  </si>
+  <si>
+    <t>https://discord.gg/teengirl</t>
+  </si>
+  <si>
+    <t>348269107151503360</t>
+  </si>
+  <si>
+    <t>https://discord.gg/pornox</t>
+  </si>
+  <si>
+    <t>850205239302946866</t>
+  </si>
+  <si>
+    <t>790040571250606092</t>
+  </si>
+  <si>
+    <t>https://discord.gg/s3xygirlsss</t>
+  </si>
+  <si>
+    <t>994010326146236546</t>
+  </si>
+  <si>
+    <t>480744971574706176</t>
+  </si>
+  <si>
+    <t>562323160222138390</t>
+  </si>
+  <si>
+    <t>https://discord.gg/egirl-paradise</t>
+  </si>
+  <si>
+    <t>1205200475214057557</t>
+  </si>
+  <si>
+    <t>1011715621865672774</t>
+  </si>
+  <si>
+    <t>1116542663634718781</t>
+  </si>
+  <si>
+    <t>776816173684621333</t>
+  </si>
+  <si>
+    <t>1169190585861677097</t>
+  </si>
+  <si>
+    <t>https://sc.link/3nzqZ</t>
+  </si>
+  <si>
+    <t>701687786914316320</t>
+  </si>
+  <si>
+    <t>https://vakmtenz.com</t>
+  </si>
+  <si>
+    <t>537683559251574796</t>
+  </si>
+  <si>
+    <t>1197457788041957388</t>
+  </si>
+  <si>
+    <t>939952037116915753</t>
+  </si>
+  <si>
+    <t>https://lstu.fr/invite</t>
+  </si>
+  <si>
+    <t>923204984168923147</t>
+  </si>
+  <si>
+    <t>933228345108348928</t>
+  </si>
+  <si>
+    <t>Crypto Fraud</t>
+  </si>
+  <si>
+    <t>https://xcoin-presale.com</t>
+  </si>
+  <si>
+    <t>799284471609556992</t>
+  </si>
+  <si>
+    <t>https://discord.gg/U3cBgqx6</t>
+  </si>
+  <si>
+    <t>423338844767911937</t>
+  </si>
+  <si>
+    <t>https://steamescommnunity.com/s/1059012495</t>
   </si>
 </sst>
 </file>
@@ -30916,426 +31123,1718 @@
       <c r="A666" s="1">
         <v>665.0</v>
       </c>
-      <c r="C666" s="6"/>
+      <c r="B666" s="2">
+        <v>45730.0</v>
+      </c>
+      <c r="C666" s="3" t="s">
+        <v>1783</v>
+      </c>
+      <c r="D666" s="1" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E666" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F666" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G666" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H666" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I666" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J666" s="4" t="s">
+        <v>1785</v>
+      </c>
+      <c r="K666" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L666" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="667">
       <c r="A667" s="1">
         <v>666.0</v>
       </c>
-      <c r="C667" s="6"/>
+      <c r="B667" s="2">
+        <v>45730.0</v>
+      </c>
+      <c r="C667" s="3" t="s">
+        <v>1786</v>
+      </c>
+      <c r="D667" s="1" t="s">
+        <v>1787</v>
+      </c>
+      <c r="E667" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F667" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G667" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H667" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I667" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J667" s="4" t="s">
+        <v>1788</v>
+      </c>
+      <c r="K667" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L667" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="668">
       <c r="A668" s="1">
         <v>667.0</v>
       </c>
-      <c r="C668" s="6"/>
+      <c r="B668" s="2">
+        <v>44417.0</v>
+      </c>
+      <c r="C668" s="3" t="s">
+        <v>1789</v>
+      </c>
+      <c r="D668" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E668" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F668" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G668" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H668" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I668" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J668" s="4" t="s">
+        <v>1791</v>
+      </c>
+      <c r="K668" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L668" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="669">
       <c r="A669" s="1">
         <v>668.0</v>
       </c>
-      <c r="C669" s="6"/>
+      <c r="B669" s="2">
+        <v>44433.0</v>
+      </c>
+      <c r="C669" s="3" t="s">
+        <v>1792</v>
+      </c>
+      <c r="D669" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E669" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F669" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G669" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H669" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I669" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J669" s="4" t="s">
+        <v>1793</v>
+      </c>
+      <c r="K669" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L669" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="670">
       <c r="A670" s="1">
         <v>669.0</v>
       </c>
-      <c r="C670" s="6"/>
+      <c r="B670" s="5">
+        <v>44516.0</v>
+      </c>
+      <c r="C670" s="3" t="s">
+        <v>1794</v>
+      </c>
+      <c r="D670" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E670" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F670" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G670" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H670" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I670" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J670" s="4" t="s">
+        <v>1795</v>
+      </c>
+      <c r="K670" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L670" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="671">
       <c r="A671" s="1">
         <v>670.0</v>
       </c>
-      <c r="C671" s="6"/>
+      <c r="B671" s="5">
+        <v>44516.0</v>
+      </c>
+      <c r="C671" s="3" t="s">
+        <v>1796</v>
+      </c>
+      <c r="D671" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E671" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F671" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G671" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H671" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I671" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J671" s="4" t="s">
+        <v>1795</v>
+      </c>
+      <c r="K671" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L671" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="672">
       <c r="A672" s="1">
         <v>671.0</v>
       </c>
-      <c r="C672" s="6"/>
+      <c r="B672" s="5">
+        <v>44519.0</v>
+      </c>
+      <c r="C672" s="3" t="s">
+        <v>1794</v>
+      </c>
+      <c r="D672" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E672" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F672" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G672" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H672" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I672" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J672" s="4" t="s">
+        <v>1797</v>
+      </c>
+      <c r="K672" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L672" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="673">
       <c r="A673" s="1">
         <v>672.0</v>
       </c>
-      <c r="C673" s="6"/>
+      <c r="B673" s="5">
+        <v>44525.0</v>
+      </c>
+      <c r="C673" s="3" t="s">
+        <v>1794</v>
+      </c>
+      <c r="D673" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E673" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F673" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G673" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H673" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I673" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J673" s="4" t="s">
+        <v>1798</v>
+      </c>
+      <c r="K673" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L673" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="674">
       <c r="A674" s="1">
         <v>673.0</v>
       </c>
-      <c r="C674" s="6"/>
+      <c r="B674" s="5">
+        <v>44525.0</v>
+      </c>
+      <c r="C674" s="3" t="s">
+        <v>1794</v>
+      </c>
+      <c r="D674" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E674" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F674" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G674" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H674" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I674" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J674" s="4" t="s">
+        <v>1798</v>
+      </c>
+      <c r="K674" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L674" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="675">
       <c r="A675" s="1">
         <v>674.0</v>
       </c>
-      <c r="C675" s="6"/>
+      <c r="B675" s="5">
+        <v>44532.0</v>
+      </c>
+      <c r="C675" s="3" t="s">
+        <v>1799</v>
+      </c>
+      <c r="D675" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E675" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F675" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G675" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H675" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I675" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J675" s="4" t="s">
+        <v>1800</v>
+      </c>
+      <c r="K675" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L675" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="676">
       <c r="A676" s="1">
         <v>675.0</v>
       </c>
-      <c r="C676" s="6"/>
+      <c r="B676" s="5">
+        <v>44573.0</v>
+      </c>
+      <c r="C676" s="3" t="s">
+        <v>1801</v>
+      </c>
+      <c r="D676" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E676" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F676" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G676" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H676" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I676" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J676" s="4" t="s">
+        <v>1802</v>
+      </c>
+      <c r="K676" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L676" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="677">
       <c r="A677" s="1">
         <v>676.0</v>
       </c>
-      <c r="C677" s="6"/>
+      <c r="B677" s="5">
+        <v>44579.0</v>
+      </c>
+      <c r="C677" s="3" t="s">
+        <v>1803</v>
+      </c>
+      <c r="D677" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E677" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F677" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G677" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H677" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I677" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J677" s="4" t="s">
+        <v>1804</v>
+      </c>
+      <c r="K677" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L677" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="678">
       <c r="A678" s="1">
         <v>677.0</v>
       </c>
-      <c r="C678" s="6"/>
+      <c r="B678" s="5">
+        <v>44593.0</v>
+      </c>
+      <c r="C678" s="3" t="s">
+        <v>1794</v>
+      </c>
+      <c r="D678" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E678" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F678" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G678" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H678" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I678" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J678" s="4" t="s">
+        <v>1805</v>
+      </c>
+      <c r="K678" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L678" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="679">
       <c r="A679" s="1">
         <v>678.0</v>
       </c>
-      <c r="C679" s="6"/>
+      <c r="B679" s="5">
+        <v>45065.0</v>
+      </c>
+      <c r="C679" s="3" t="s">
+        <v>1806</v>
+      </c>
+      <c r="D679" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E679" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F679" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G679" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H679" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I679" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J679" s="4" t="s">
+        <v>1807</v>
+      </c>
+      <c r="K679" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L679" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="680">
       <c r="A680" s="1">
         <v>679.0</v>
       </c>
-      <c r="C680" s="6"/>
+      <c r="B680" s="5">
+        <v>45114.0</v>
+      </c>
+      <c r="C680" s="3" t="s">
+        <v>1808</v>
+      </c>
+      <c r="D680" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E680" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F680" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G680" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H680" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I680" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J680" s="4" t="s">
+        <v>1809</v>
+      </c>
+      <c r="K680" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L680" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="681">
       <c r="A681" s="1">
         <v>680.0</v>
       </c>
-      <c r="C681" s="6"/>
+      <c r="B681" s="5">
+        <v>45133.0</v>
+      </c>
+      <c r="C681" s="3" t="s">
+        <v>1810</v>
+      </c>
+      <c r="D681" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E681" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F681" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G681" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H681" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I681" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J681" s="4" t="s">
+        <v>1811</v>
+      </c>
+      <c r="K681" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L681" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="682">
       <c r="A682" s="1">
         <v>681.0</v>
       </c>
-      <c r="C682" s="6"/>
+      <c r="B682" s="5">
+        <v>45214.0</v>
+      </c>
+      <c r="C682" s="3" t="s">
+        <v>1812</v>
+      </c>
+      <c r="D682" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E682" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F682" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G682" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H682" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I682" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J682" s="4" t="s">
+        <v>1813</v>
+      </c>
+      <c r="K682" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L682" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="683">
       <c r="A683" s="1">
         <v>682.0</v>
       </c>
-      <c r="C683" s="6"/>
+      <c r="B683" s="2">
+        <v>45341.0</v>
+      </c>
+      <c r="C683" s="3" t="s">
+        <v>1814</v>
+      </c>
+      <c r="D683" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E683" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F683" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G683" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H683" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I683" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J683" s="4" t="s">
+        <v>1815</v>
+      </c>
+      <c r="K683" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L683" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="684">
       <c r="A684" s="1">
         <v>683.0</v>
       </c>
-      <c r="C684" s="6"/>
+      <c r="B684" s="2">
+        <v>45346.0</v>
+      </c>
+      <c r="C684" s="3" t="s">
+        <v>1816</v>
+      </c>
+      <c r="D684" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E684" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F684" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G684" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H684" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I684" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J684" s="4" t="s">
+        <v>1817</v>
+      </c>
+      <c r="K684" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L684" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="685">
       <c r="A685" s="1">
         <v>684.0</v>
       </c>
-      <c r="C685" s="6"/>
+      <c r="B685" s="2">
+        <v>45347.0</v>
+      </c>
+      <c r="C685" s="3" t="s">
+        <v>1818</v>
+      </c>
+      <c r="D685" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E685" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F685" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G685" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H685" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I685" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J685" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="K685" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L685" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="686">
       <c r="A686" s="1">
         <v>685.0</v>
       </c>
-      <c r="C686" s="6"/>
+      <c r="B686" s="2">
+        <v>45369.0</v>
+      </c>
+      <c r="C686" s="3" t="s">
+        <v>1819</v>
+      </c>
+      <c r="D686" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E686" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F686" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G686" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H686" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I686" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J686" s="4" t="s">
+        <v>1820</v>
+      </c>
+      <c r="K686" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L686" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="687">
       <c r="A687" s="1">
         <v>686.0</v>
       </c>
-      <c r="C687" s="6"/>
+      <c r="B687" s="2">
+        <v>45392.0</v>
+      </c>
+      <c r="C687" s="3" t="s">
+        <v>1821</v>
+      </c>
+      <c r="D687" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E687" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F687" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G687" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H687" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I687" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J687" s="4" t="s">
+        <v>1822</v>
+      </c>
+      <c r="K687" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L687" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="688">
       <c r="A688" s="1">
         <v>687.0</v>
       </c>
-      <c r="C688" s="6"/>
+      <c r="B688" s="2">
+        <v>45397.0</v>
+      </c>
+      <c r="C688" s="3" t="s">
+        <v>1823</v>
+      </c>
+      <c r="D688" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E688" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F688" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G688" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H688" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I688" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J688" s="4" t="s">
+        <v>1824</v>
+      </c>
+      <c r="K688" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L688" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="689">
       <c r="A689" s="1">
         <v>688.0</v>
       </c>
-      <c r="C689" s="6"/>
+      <c r="B689" s="2">
+        <v>45398.0</v>
+      </c>
+      <c r="C689" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="D689" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E689" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F689" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G689" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H689" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I689" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J689" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="K689" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L689" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="690">
       <c r="A690" s="1">
         <v>689.0</v>
       </c>
-      <c r="C690" s="6"/>
+      <c r="B690" s="2">
+        <v>45401.0</v>
+      </c>
+      <c r="C690" s="3" t="s">
+        <v>1825</v>
+      </c>
+      <c r="D690" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E690" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F690" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G690" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H690" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I690" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J690" s="4" t="s">
+        <v>759</v>
+      </c>
+      <c r="K690" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L690" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="691">
       <c r="A691" s="1">
         <v>690.0</v>
       </c>
-      <c r="C691" s="6"/>
+      <c r="B691" s="2">
+        <v>45405.0</v>
+      </c>
+      <c r="C691" s="3" t="s">
+        <v>1826</v>
+      </c>
+      <c r="D691" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E691" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F691" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G691" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H691" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I691" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J691" s="4" t="s">
+        <v>1827</v>
+      </c>
+      <c r="K691" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L691" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="692">
       <c r="A692" s="1">
         <v>691.0</v>
       </c>
-      <c r="C692" s="6"/>
+      <c r="B692" s="2">
+        <v>45412.0</v>
+      </c>
+      <c r="C692" s="3" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D692" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E692" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F692" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G692" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H692" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I692" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J692" s="4" t="s">
+        <v>832</v>
+      </c>
+      <c r="K692" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L692" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="693">
       <c r="A693" s="1">
         <v>692.0</v>
       </c>
-      <c r="C693" s="6"/>
+      <c r="B693" s="2">
+        <v>45420.0</v>
+      </c>
+      <c r="C693" s="3" t="s">
+        <v>1829</v>
+      </c>
+      <c r="D693" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E693" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F693" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G693" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H693" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I693" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J693" s="4" t="s">
+        <v>874</v>
+      </c>
+      <c r="K693" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L693" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="694">
       <c r="A694" s="1">
         <v>693.0</v>
       </c>
-      <c r="C694" s="6"/>
+      <c r="B694" s="2">
+        <v>45446.0</v>
+      </c>
+      <c r="C694" s="3" t="s">
+        <v>1830</v>
+      </c>
+      <c r="D694" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E694" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F694" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G694" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H694" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I694" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J694" s="4" t="s">
+        <v>1831</v>
+      </c>
+      <c r="K694" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L694" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="695">
       <c r="A695" s="1">
         <v>694.0</v>
       </c>
-      <c r="C695" s="6"/>
+      <c r="B695" s="2">
+        <v>45461.0</v>
+      </c>
+      <c r="C695" s="3" t="s">
+        <v>1832</v>
+      </c>
+      <c r="D695" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E695" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F695" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G695" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H695" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I695" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J695" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="K695" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L695" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="696">
       <c r="A696" s="1">
         <v>695.0</v>
       </c>
-      <c r="C696" s="6"/>
+      <c r="B696" s="2">
+        <v>45464.0</v>
+      </c>
+      <c r="C696" s="3" t="s">
+        <v>1833</v>
+      </c>
+      <c r="D696" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E696" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F696" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G696" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H696" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I696" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J696" s="4" t="s">
+        <v>1221</v>
+      </c>
+      <c r="K696" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L696" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="697">
       <c r="A697" s="1">
         <v>696.0</v>
       </c>
-      <c r="C697" s="6"/>
+      <c r="B697" s="2">
+        <v>45475.0</v>
+      </c>
+      <c r="C697" s="3" t="s">
+        <v>1834</v>
+      </c>
+      <c r="D697" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E697" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F697" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G697" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H697" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I697" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J697" s="4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="K697" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L697" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="698">
       <c r="A698" s="1">
         <v>697.0</v>
       </c>
-      <c r="C698" s="6"/>
+      <c r="B698" s="2">
+        <v>45483.0</v>
+      </c>
+      <c r="C698" s="3" t="s">
+        <v>1835</v>
+      </c>
+      <c r="D698" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E698" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F698" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G698" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H698" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I698" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J698" s="4" t="s">
+        <v>1349</v>
+      </c>
+      <c r="K698" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L698" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="699">
       <c r="A699" s="1">
         <v>698.0</v>
       </c>
-      <c r="C699" s="6"/>
+      <c r="B699" s="2">
+        <v>45494.0</v>
+      </c>
+      <c r="C699" s="3" t="s">
+        <v>1836</v>
+      </c>
+      <c r="D699" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E699" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F699" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G699" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H699" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I699" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J699" s="4" t="s">
+        <v>1837</v>
+      </c>
+      <c r="K699" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L699" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="700">
       <c r="A700" s="1">
         <v>699.0</v>
       </c>
-      <c r="C700" s="6"/>
+      <c r="B700" s="2">
+        <v>45503.0</v>
+      </c>
+      <c r="C700" s="3" t="s">
+        <v>1838</v>
+      </c>
+      <c r="D700" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E700" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F700" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G700" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H700" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I700" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J700" s="4" t="s">
+        <v>1839</v>
+      </c>
+      <c r="K700" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L700" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="701">
       <c r="A701" s="1">
         <v>700.0</v>
       </c>
-      <c r="C701" s="6"/>
+      <c r="B701" s="2">
+        <v>45523.0</v>
+      </c>
+      <c r="C701" s="3" t="s">
+        <v>1840</v>
+      </c>
+      <c r="D701" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E701" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F701" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G701" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H701" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I701" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J701" s="4" t="s">
+        <v>1432</v>
+      </c>
+      <c r="K701" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L701" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="702">
       <c r="A702" s="1">
         <v>701.0</v>
       </c>
-      <c r="C702" s="6"/>
+      <c r="B702" s="2">
+        <v>45538.0</v>
+      </c>
+      <c r="C702" s="3" t="s">
+        <v>1841</v>
+      </c>
+      <c r="D702" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E702" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F702" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G702" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H702" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I702" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J702" s="4" t="s">
+        <v>1448</v>
+      </c>
+      <c r="K702" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L702" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="703">
       <c r="A703" s="1">
         <v>702.0</v>
       </c>
-      <c r="C703" s="6"/>
+      <c r="B703" s="5">
+        <v>45612.0</v>
+      </c>
+      <c r="C703" s="3" t="s">
+        <v>1842</v>
+      </c>
+      <c r="D703" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E703" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F703" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G703" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H703" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I703" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J703" s="4" t="s">
+        <v>1843</v>
+      </c>
+      <c r="K703" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L703" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="704">
       <c r="A704" s="1">
         <v>703.0</v>
       </c>
-      <c r="C704" s="6"/>
+      <c r="B704" s="5">
+        <v>45645.0</v>
+      </c>
+      <c r="C704" s="3" t="s">
+        <v>1844</v>
+      </c>
+      <c r="D704" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E704" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F704" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G704" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H704" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I704" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J704" s="4" t="s">
+        <v>1534</v>
+      </c>
+      <c r="K704" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L704" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="705">
       <c r="A705" s="1">
         <v>704.0</v>
       </c>
-      <c r="C705" s="6"/>
+      <c r="B705" s="2">
+        <v>45685.0</v>
+      </c>
+      <c r="C705" s="3" t="s">
+        <v>1845</v>
+      </c>
+      <c r="D705" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E705" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F705" s="1" t="s">
+        <v>1846</v>
+      </c>
+      <c r="G705" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H705" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I705" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="J705" s="4" t="s">
+        <v>1847</v>
+      </c>
+      <c r="K705" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L705" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="706">
       <c r="A706" s="1">
         <v>705.0</v>
       </c>
-      <c r="C706" s="6"/>
+      <c r="B706" s="2">
+        <v>45700.0</v>
+      </c>
+      <c r="C706" s="3" t="s">
+        <v>1848</v>
+      </c>
+      <c r="D706" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E706" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F706" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G706" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H706" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I706" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J706" s="4" t="s">
+        <v>1849</v>
+      </c>
+      <c r="K706" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L706" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="707">
       <c r="A707" s="1">
         <v>706.0</v>
       </c>
-      <c r="C707" s="6"/>
+      <c r="B707" s="2">
+        <v>45705.0</v>
+      </c>
+      <c r="C707" s="3" t="s">
+        <v>1850</v>
+      </c>
+      <c r="D707" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E707" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F707" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G707" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H707" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I707" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J707" s="4" t="s">
+        <v>1851</v>
+      </c>
+      <c r="K707" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L707" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="708">
       <c r="A708" s="1">
         <v>707.0</v>
       </c>
-      <c r="C708" s="6"/>
+      <c r="B708" s="2">
+        <v>45728.0</v>
+      </c>
+      <c r="C708" s="3" t="s">
+        <v>1777</v>
+      </c>
+      <c r="D708" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E708" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F708" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G708" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H708" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I708" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J708" s="4" t="s">
+        <v>1779</v>
+      </c>
+      <c r="K708" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L708" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="709">
-      <c r="A709" s="1">
-        <v>708.0</v>
-      </c>
       <c r="C709" s="6"/>
     </row>
     <row r="710">
-      <c r="A710" s="1">
-        <v>709.0</v>
-      </c>
       <c r="C710" s="6"/>
     </row>
     <row r="711">
-      <c r="A711" s="1">
-        <v>710.0</v>
-      </c>
       <c r="C711" s="6"/>
     </row>
     <row r="712">
-      <c r="A712" s="1">
-        <v>711.0</v>
-      </c>
       <c r="C712" s="6"/>
     </row>
     <row r="713">
-      <c r="A713" s="1">
-        <v>712.0</v>
-      </c>
       <c r="C713" s="6"/>
     </row>
     <row r="714">
-      <c r="A714" s="1">
-        <v>713.0</v>
-      </c>
       <c r="C714" s="6"/>
     </row>
     <row r="715">
-      <c r="A715" s="1">
-        <v>714.0</v>
-      </c>
       <c r="C715" s="6"/>
     </row>
     <row r="716">
-      <c r="A716" s="1">
-        <v>715.0</v>
-      </c>
       <c r="C716" s="6"/>
     </row>
     <row r="717">
-      <c r="A717" s="1">
-        <v>716.0</v>
-      </c>
       <c r="C717" s="6"/>
     </row>
     <row r="718">
-      <c r="A718" s="1">
-        <v>717.0</v>
-      </c>
       <c r="C718" s="6"/>
     </row>
     <row r="719">
-      <c r="A719" s="1">
-        <v>718.0</v>
-      </c>
       <c r="C719" s="6"/>
     </row>
     <row r="720">
-      <c r="A720" s="1">
-        <v>719.0</v>
-      </c>
       <c r="C720" s="6"/>
     </row>
     <row r="721">
-      <c r="A721" s="1">
-        <v>720.0</v>
-      </c>
       <c r="C721" s="6"/>
     </row>
     <row r="722">
-      <c r="A722" s="1">
-        <v>721.0</v>
-      </c>
       <c r="C722" s="6"/>
     </row>
     <row r="723">
-      <c r="A723" s="1">
-        <v>722.0</v>
-      </c>
       <c r="C723" s="6"/>
     </row>
     <row r="724">
-      <c r="A724" s="1">
-        <v>723.0</v>
-      </c>
       <c r="C724" s="6"/>
     </row>
     <row r="725">
-      <c r="A725" s="1">
-        <v>724.0</v>
-      </c>
       <c r="C725" s="6"/>
     </row>
     <row r="726">
-      <c r="A726" s="1">
-        <v>725.0</v>
-      </c>
       <c r="C726" s="6"/>
     </row>
     <row r="727">
-      <c r="A727" s="1">
-        <v>726.0</v>
-      </c>
       <c r="C727" s="6"/>
     </row>
     <row r="728">
-      <c r="A728" s="1">
-        <v>727.0</v>
-      </c>
       <c r="C728" s="6"/>
     </row>
     <row r="729">
-      <c r="A729" s="1">
-        <v>728.0</v>
-      </c>
       <c r="C729" s="6"/>
     </row>
     <row r="730">
-      <c r="A730" s="1">
-        <v>729.0</v>
-      </c>
       <c r="C730" s="6"/>
     </row>
     <row r="731">
-      <c r="A731" s="1">
-        <v>730.0</v>
-      </c>
       <c r="C731" s="6"/>
     </row>
     <row r="732">
-      <c r="A732" s="1">
-        <v>731.0</v>
-      </c>
       <c r="C732" s="6"/>
     </row>
     <row r="733">
-      <c r="A733" s="1">
-        <v>732.0</v>
-      </c>
       <c r="C733" s="6"/>
     </row>
     <row r="734">
-      <c r="A734" s="1">
-        <v>733.0</v>
-      </c>
       <c r="C734" s="6"/>
     </row>
     <row r="735">
-      <c r="A735" s="1">
-        <v>734.0</v>
-      </c>
       <c r="C735" s="6"/>
     </row>
     <row r="736">
-      <c r="A736" s="1">
-        <v>735.0</v>
-      </c>
       <c r="C736" s="6"/>
     </row>
   </sheetData>
@@ -32003,7 +33502,50 @@
     <hyperlink r:id="rId661" ref="J663"/>
     <hyperlink r:id="rId662" ref="J664"/>
     <hyperlink r:id="rId663" ref="J665"/>
+    <hyperlink r:id="rId664" ref="J666"/>
+    <hyperlink r:id="rId665" ref="J667"/>
+    <hyperlink r:id="rId666" ref="J668"/>
+    <hyperlink r:id="rId667" ref="J669"/>
+    <hyperlink r:id="rId668" ref="J670"/>
+    <hyperlink r:id="rId669" ref="J671"/>
+    <hyperlink r:id="rId670" ref="J672"/>
+    <hyperlink r:id="rId671" ref="J673"/>
+    <hyperlink r:id="rId672" ref="J674"/>
+    <hyperlink r:id="rId673" ref="J675"/>
+    <hyperlink r:id="rId674" ref="J676"/>
+    <hyperlink r:id="rId675" ref="J677"/>
+    <hyperlink r:id="rId676" ref="J678"/>
+    <hyperlink r:id="rId677" ref="J679"/>
+    <hyperlink r:id="rId678" ref="J680"/>
+    <hyperlink r:id="rId679" ref="J681"/>
+    <hyperlink r:id="rId680" ref="J682"/>
+    <hyperlink r:id="rId681" ref="J683"/>
+    <hyperlink r:id="rId682" ref="J684"/>
+    <hyperlink r:id="rId683" ref="J685"/>
+    <hyperlink r:id="rId684" ref="J686"/>
+    <hyperlink r:id="rId685" ref="J687"/>
+    <hyperlink r:id="rId686" ref="J688"/>
+    <hyperlink r:id="rId687" ref="J689"/>
+    <hyperlink r:id="rId688" ref="J690"/>
+    <hyperlink r:id="rId689" ref="J691"/>
+    <hyperlink r:id="rId690" ref="J692"/>
+    <hyperlink r:id="rId691" ref="J693"/>
+    <hyperlink r:id="rId692" ref="J694"/>
+    <hyperlink r:id="rId693" ref="J695"/>
+    <hyperlink r:id="rId694" ref="J696"/>
+    <hyperlink r:id="rId695" ref="J697"/>
+    <hyperlink r:id="rId696" ref="J698"/>
+    <hyperlink r:id="rId697" ref="J699"/>
+    <hyperlink r:id="rId698" ref="J700"/>
+    <hyperlink r:id="rId699" ref="J701"/>
+    <hyperlink r:id="rId700" ref="J702"/>
+    <hyperlink r:id="rId701" ref="J703"/>
+    <hyperlink r:id="rId702" ref="J704"/>
+    <hyperlink r:id="rId703" ref="J705"/>
+    <hyperlink r:id="rId704" ref="J706"/>
+    <hyperlink r:id="rId705" ref="J707"/>
+    <hyperlink r:id="rId706" ref="J708"/>
   </hyperlinks>
-  <drawing r:id="rId664"/>
+  <drawing r:id="rId707"/>
 </worksheet>
 </file>
</xml_diff>